<commit_message>
CHECKPOINT: before changing to second way
</commit_message>
<xml_diff>
--- a/StatData.xlsx
+++ b/StatData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6786443F-8A92-4026-A2F6-7854787B1D13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7647AA56-60E9-4B8F-A725-95700213B94F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Season" sheetId="5" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="710">
   <si>
     <t>T</t>
   </si>
@@ -2137,7 +2137,16 @@
     <t>RUNS_ALLOWED</t>
   </si>
   <si>
-    <t>DID_NOT_PLAY</t>
+    <t>DOUBLE_PLAY</t>
+  </si>
+  <si>
+    <t>NUMBER(5,3)</t>
+  </si>
+  <si>
+    <t>NUMBER(5,0)</t>
+  </si>
+  <si>
+    <t>NUMBER(5,2)</t>
   </si>
 </sst>
 </file>
@@ -2549,7 +2558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31E251B-FF08-4194-95F7-3D0B4FF46B3A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2586,7 +2595,7 @@
   <dimension ref="A1:AB115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2623,10 +2632,58 @@
       <c r="B1" t="s">
         <v>669</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -12417,8 +12474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12453,6 +12510,51 @@
       <c r="B1" t="s">
         <v>669</v>
       </c>
+      <c r="G1" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>707</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">

</xml_diff>